<commit_message>
add to project examples of unput and output data
</commit_message>
<xml_diff>
--- a/test_data/multiple_product/test_data_5x12.xlsx
+++ b/test_data/multiple_product/test_data_5x12.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1DB0BE-C4A8-4DD7-94C0-E43B275202BE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBA5302-1F98-4B4D-8E32-345DF76A5E37}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="50">
   <si>
     <t>жд</t>
   </si>
@@ -137,13 +138,7 @@
     <t>Считать стоимость за рейс или за тонну, если за рейс то 1, если за тонну, то 0</t>
   </si>
   <si>
-    <t>картофель</t>
-  </si>
-  <si>
     <t>В чем дать ответ</t>
-  </si>
-  <si>
-    <t>trips</t>
   </si>
   <si>
     <t>Какой моделью решать</t>
@@ -152,16 +147,31 @@
     <t>fractional</t>
   </si>
   <si>
-    <t>Решать вместе с другими продуктами в группе</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>По какому параметру оптимизировать</t>
   </si>
   <si>
     <t>cost</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>помидор</t>
+  </si>
+  <si>
+    <t>Макс. Стоимость</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>Приоритет</t>
+  </si>
+  <si>
+    <t>Товары, по которым решение должно проводиться вместе</t>
+  </si>
+  <si>
+    <t>мука, помидор</t>
   </si>
 </sst>
 </file>
@@ -588,7 +598,7 @@
   <dimension ref="A1:AP49"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:S1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,28 +623,10 @@
         <v>1440</v>
       </c>
       <c r="J1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P1" t="s">
         <v>43</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" t="s">
-        <v>45</v>
-      </c>
-      <c r="S1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.25">
@@ -3032,8 +3024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D03F1B94-45E1-4DD4-9751-8C4333E5ED27}">
   <dimension ref="A1:AP49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3043,7 +3035,7 @@
         <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
         <v>35</v>
@@ -3058,28 +3050,10 @@
         <v>1440</v>
       </c>
       <c r="J1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P1" t="s">
         <v>43</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" t="s">
-        <v>45</v>
-      </c>
-      <c r="S1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.25">
@@ -5471,4 +5445,55 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7466710-BFF6-4C75-A7FC-E9956B1723BA}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>